<commit_message>
More modules in DB, updated GUI for split AI/AO types
</commit_message>
<xml_diff>
--- a/PC3 Features.xlsx
+++ b/PC3 Features.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05941AFD-B6C3-475C-A7F9-949E93366D3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{05941AFD-B6C3-475C-A7F9-949E93366D3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{7AAA5025-2A01-47F6-A36B-1FDE1BA1C377}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1288,7 +1288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1362,22 +1362,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1389,16 +1374,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1412,6 +1412,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1754,10 +1757,10 @@
   <dimension ref="A1:BN15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AH3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W3" sqref="W3"/>
+      <selection pane="bottomRight" activeCell="BC2" sqref="BC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,84 +1772,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="28" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="29" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="36" t="s">
         <v>309</v>
       </c>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="29"/>
-      <c r="AQ1" s="29"/>
-      <c r="AR1" s="29"/>
-      <c r="AS1" s="29"/>
-      <c r="AT1" s="29"/>
-      <c r="AU1" s="29"/>
-      <c r="AV1" s="29"/>
-      <c r="AW1" s="29"/>
-      <c r="AX1" s="29"/>
-      <c r="AY1" s="29"/>
-      <c r="AZ1" s="29"/>
-      <c r="BA1" s="29"/>
-      <c r="BB1" s="29"/>
-      <c r="BC1" s="29"/>
-      <c r="BD1" s="29"/>
-      <c r="BE1" s="29"/>
-      <c r="BF1" s="29"/>
-      <c r="BG1" s="29"/>
-      <c r="BH1" s="29"/>
-      <c r="BI1" s="29"/>
-      <c r="BJ1" s="29"/>
-      <c r="BK1" s="29"/>
-      <c r="BL1" s="29"/>
-      <c r="BM1" s="29"/>
-      <c r="BN1" s="29"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36"/>
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="36"/>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="36"/>
+      <c r="AU1" s="36"/>
+      <c r="AV1" s="36"/>
+      <c r="AW1" s="36"/>
+      <c r="AX1" s="36"/>
+      <c r="AY1" s="36"/>
+      <c r="AZ1" s="36"/>
+      <c r="BA1" s="36"/>
+      <c r="BB1" s="36"/>
+      <c r="BC1" s="36"/>
+      <c r="BD1" s="36"/>
+      <c r="BE1" s="36"/>
+      <c r="BF1" s="36"/>
+      <c r="BG1" s="36"/>
+      <c r="BH1" s="36"/>
+      <c r="BI1" s="36"/>
+      <c r="BJ1" s="36"/>
+      <c r="BK1" s="36"/>
+      <c r="BL1" s="36"/>
+      <c r="BM1" s="36"/>
+      <c r="BN1" s="36"/>
     </row>
     <row r="2" spans="1:66" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
@@ -1910,31 +1913,31 @@
       <c r="W2" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="X2" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Y2" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="12" t="s">
+      <c r="Z2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AA2" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="12" t="s">
+      <c r="AB2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AC2" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="12" t="s">
+      <c r="AD2" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="12" t="s">
+      <c r="AE2" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="AF2" s="12" t="s">
+      <c r="AF2" s="44" t="s">
         <v>33</v>
       </c>
       <c r="AG2" s="12" t="s">
@@ -1943,16 +1946,16 @@
       <c r="AH2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AI2" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="AJ2" s="12" t="s">
+      <c r="AJ2" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="AK2" s="12" t="s">
+      <c r="AK2" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="AL2" s="12" t="s">
+      <c r="AL2" s="44" t="s">
         <v>39</v>
       </c>
       <c r="AM2" s="12" t="s">
@@ -1964,13 +1967,13 @@
       <c r="AO2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AP2" s="12" t="s">
+      <c r="AP2" s="44" t="s">
         <v>43</v>
       </c>
       <c r="AQ2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AR2" s="12" t="s">
+      <c r="AR2" s="44" t="s">
         <v>45</v>
       </c>
       <c r="AS2" s="12" t="s">
@@ -1979,7 +1982,7 @@
       <c r="AT2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AU2" s="12" t="s">
+      <c r="AU2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="AV2" s="12" t="s">
@@ -1988,7 +1991,7 @@
       <c r="AW2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AX2" s="12" t="s">
+      <c r="AX2" s="44" t="s">
         <v>51</v>
       </c>
       <c r="AY2" s="12" t="s">
@@ -1997,13 +2000,13 @@
       <c r="AZ2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="BA2" s="12" t="s">
+      <c r="BA2" s="44" t="s">
         <v>54</v>
       </c>
       <c r="BB2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="BC2" s="12" t="s">
+      <c r="BC2" s="44" t="s">
         <v>56</v>
       </c>
       <c r="BD2" s="12" t="s">
@@ -2041,7 +2044,7 @@
       </c>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2049,15 +2052,15 @@
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="31">
+      <c r="E3" s="27">
         <v>3</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="31">
+      <c r="G3" s="27">
         <v>10</v>
       </c>
       <c r="H3" s="8"/>
-      <c r="I3" s="31">
+      <c r="I3" s="27">
         <v>5</v>
       </c>
       <c r="J3" s="8"/>
@@ -2066,7 +2069,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
-      <c r="P3" s="31">
+      <c r="P3" s="27">
         <v>30</v>
       </c>
       <c r="Q3" s="8"/>
@@ -2123,17 +2126,17 @@
       <c r="BN3" s="13"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="33"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="33"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="33"/>
+      <c r="I4" s="28"/>
       <c r="J4" s="5">
         <v>5</v>
       </c>
@@ -2144,7 +2147,7 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-      <c r="P4" s="33"/>
+      <c r="P4" s="28"/>
       <c r="Q4" s="40">
         <v>4</v>
       </c>
@@ -2199,7 +2202,7 @@
       <c r="BN4" s="25"/>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="33" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2208,7 +2211,7 @@
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="31">
+      <c r="F5" s="27">
         <v>12</v>
       </c>
       <c r="G5" s="8"/>
@@ -2225,21 +2228,21 @@
       <c r="P5" s="5">
         <v>12</v>
       </c>
-      <c r="Q5" s="34">
+      <c r="Q5" s="29">
         <v>13</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="31">
+      <c r="R5" s="30"/>
+      <c r="S5" s="27">
         <v>15</v>
       </c>
-      <c r="T5" s="31">
+      <c r="T5" s="27">
         <v>28</v>
       </c>
-      <c r="U5" s="31">
+      <c r="U5" s="27">
         <v>3</v>
       </c>
       <c r="V5" s="10"/>
-      <c r="W5" s="31">
+      <c r="W5" s="27">
         <v>45</v>
       </c>
       <c r="X5" s="13"/>
@@ -2287,7 +2290,7 @@
       <c r="BN5" s="26"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -2296,7 +2299,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="32"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -2313,13 +2316,13 @@
       <c r="P6" s="7">
         <v>10</v>
       </c>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="33"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="28"/>
       <c r="V6" s="11"/>
-      <c r="W6" s="32"/>
+      <c r="W6" s="37"/>
       <c r="X6" s="25"/>
       <c r="Y6" s="25"/>
       <c r="Z6" s="25"/>
@@ -2365,7 +2368,7 @@
       <c r="BN6" s="25"/>
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2374,30 +2377,30 @@
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="32"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
-      <c r="M7" s="34">
+      <c r="M7" s="29">
         <v>5</v>
       </c>
-      <c r="N7" s="35"/>
-      <c r="O7" s="31">
+      <c r="N7" s="30"/>
+      <c r="O7" s="27">
         <v>7</v>
       </c>
-      <c r="P7" s="31">
+      <c r="P7" s="27">
         <v>20</v>
       </c>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
       <c r="U7" s="8"/>
       <c r="V7" s="10"/>
-      <c r="W7" s="32"/>
+      <c r="W7" s="37"/>
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
@@ -2443,7 +2446,7 @@
       <c r="BN7" s="26"/>
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -2452,7 +2455,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="33"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -2463,17 +2466,17 @@
       <c r="L8" s="5">
         <v>5</v>
       </c>
-      <c r="M8" s="38"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="33"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
       <c r="U8" s="8"/>
       <c r="V8" s="10"/>
-      <c r="W8" s="33"/>
+      <c r="W8" s="28"/>
       <c r="X8" s="25"/>
       <c r="Y8" s="25"/>
       <c r="Z8" s="25"/>
@@ -2582,12 +2585,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="M1:W1"/>
     <mergeCell ref="X1:BN1"/>
@@ -2604,6 +2601,12 @@
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="P3:P4"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>